<commit_message>
updated country_reference data import
</commit_message>
<xml_diff>
--- a/import_data/Country Reference.xlsx
+++ b/import_data/Country Reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="527" documentId="8_{257A556D-967E-4209-9D33-134C84136F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE93682E-9C21-496C-8E94-4EF35A47671E}"/>
+  <xr:revisionPtr revIDLastSave="531" documentId="8_{257A556D-967E-4209-9D33-134C84136F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF69F6FC-EABA-45F1-AA6C-B7FA64A28BA4}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{399614B1-7431-4F70-9F99-85E1D48DE75C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="546">
   <si>
     <t>Country</t>
   </si>
@@ -1558,9 +1558,6 @@
   </si>
   <si>
     <t>UKR</t>
-  </si>
-  <si>
-    <t>bis 2018</t>
   </si>
   <si>
     <t>United Arab Emirates</t>
@@ -2053,11 +2050,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1954D66-C5CD-46D1-9EF7-0FDF3E8129B2}">
-  <dimension ref="A1:H250"/>
+  <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2206,7 +2203,7 @@
         <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -2298,7 +2295,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -2413,7 +2410,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
@@ -2528,7 +2525,7 @@
         <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
@@ -2689,12 +2686,12 @@
         <v>11</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B28" t="s">
         <v>86</v>
@@ -2896,7 +2893,7 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
@@ -3011,7 +3008,7 @@
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
@@ -3241,7 +3238,7 @@
         <v>27</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.5">
@@ -3264,7 +3261,7 @@
         <v>27</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.5">
@@ -3356,7 +3353,7 @@
         <v>27</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.5">
@@ -3540,7 +3537,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.5">
@@ -3844,7 +3841,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B78" t="s">
         <v>191</v>
@@ -3908,7 +3905,7 @@
         <v>27</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.5">
@@ -4000,7 +3997,7 @@
         <v>27</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.5">
@@ -4023,7 +4020,7 @@
         <v>23</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.5">
@@ -4092,7 +4089,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.5">
@@ -4207,7 +4204,7 @@
         <v>37</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.5">
@@ -4276,7 +4273,7 @@
         <v>27</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.5">
@@ -4437,7 +4434,7 @@
         <v>27</v>
       </c>
       <c r="G103" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.5">
@@ -4575,7 +4572,7 @@
         <v>11</v>
       </c>
       <c r="G109" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.5">
@@ -4874,7 +4871,7 @@
         <v>27</v>
       </c>
       <c r="G122" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.5">
@@ -4943,7 +4940,7 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.5">
@@ -5196,7 +5193,7 @@
         <v>11</v>
       </c>
       <c r="G136" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.5">
@@ -5219,7 +5216,7 @@
         <v>11</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.5">
@@ -5288,7 +5285,7 @@
         <v>27</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.5">
@@ -5426,7 +5423,7 @@
         <v>27</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.5">
@@ -5472,7 +5469,7 @@
         <v>11</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.5">
@@ -5587,7 +5584,7 @@
         <v>11</v>
       </c>
       <c r="G153" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.5">
@@ -5633,7 +5630,7 @@
         <v>27</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.5">
@@ -5656,7 +5653,7 @@
         <v>11</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.5">
@@ -5702,7 +5699,7 @@
         <v>27</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.5">
@@ -5725,7 +5722,7 @@
         <v>27</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.5">
@@ -5817,7 +5814,7 @@
         <v>27</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.5">
@@ -5840,7 +5837,7 @@
         <v>27</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.5">
@@ -5886,7 +5883,7 @@
         <v>27</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.5">
@@ -5955,7 +5952,7 @@
         <v>11</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.5">
@@ -5978,7 +5975,7 @@
         <v>27</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.5">
@@ -6024,7 +6021,7 @@
         <v>27</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.5">
@@ -6093,7 +6090,7 @@
         <v>11</v>
       </c>
       <c r="G175" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.5">
@@ -6116,7 +6113,7 @@
         <v>27</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.5">
@@ -6392,7 +6389,7 @@
         <v>23</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.5">
@@ -6443,7 +6440,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A191" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B191" t="s">
         <v>422</v>
@@ -6530,7 +6527,7 @@
         <v>27</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.5">
@@ -6583,6 +6580,9 @@
       <c r="A197" t="s">
         <v>433</v>
       </c>
+      <c r="B197" t="s">
+        <v>510</v>
+      </c>
       <c r="C197">
         <v>680</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>23</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.5">
@@ -6734,12 +6734,12 @@
         <v>11</v>
       </c>
       <c r="G203" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A204" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B204" t="s">
         <v>446</v>
@@ -6757,7 +6757,7 @@
         <v>37</v>
       </c>
       <c r="G204" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.5">
@@ -6826,7 +6826,7 @@
         <v>27</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.5">
@@ -6964,7 +6964,7 @@
         <v>11</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.5">
@@ -7171,7 +7171,7 @@
         <v>11</v>
       </c>
       <c r="G222" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
         <v>11</v>
       </c>
       <c r="G223" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.5">
@@ -7220,7 +7220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A225" t="s">
         <v>487</v>
       </c>
@@ -7240,10 +7240,10 @@
         <v>27</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A226" t="s">
         <v>489</v>
       </c>
@@ -7263,10 +7263,10 @@
         <v>27</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A227" t="s">
         <v>491</v>
       </c>
@@ -7286,10 +7286,10 @@
         <v>37</v>
       </c>
       <c r="G227" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.5">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A228" t="s">
         <v>493</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A229" t="s">
         <v>495</v>
       </c>
@@ -7332,10 +7332,10 @@
         <v>11</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A230" t="s">
         <v>497</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A231" t="s">
         <v>499</v>
       </c>
@@ -7378,10 +7378,10 @@
         <v>37</v>
       </c>
       <c r="G231" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.5">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A232" t="s">
         <v>501</v>
       </c>
@@ -7401,10 +7401,10 @@
         <v>27</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A233" t="s">
         <v>503</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A234" t="s">
         <v>505</v>
       </c>
@@ -7449,16 +7449,13 @@
       <c r="G234" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H234" t="s">
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A235" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A235" t="s">
+      <c r="B235" t="s">
         <v>508</v>
-      </c>
-      <c r="B235" t="s">
-        <v>509</v>
       </c>
       <c r="C235">
         <v>784</v>
@@ -7476,12 +7473,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A236" t="s">
+        <v>509</v>
+      </c>
+      <c r="B236" t="s">
         <v>510</v>
-      </c>
-      <c r="B236" t="s">
-        <v>511</v>
       </c>
       <c r="C236">
         <v>826</v>
@@ -7499,12 +7496,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A237" t="s">
+        <v>511</v>
+      </c>
+      <c r="B237" t="s">
         <v>512</v>
-      </c>
-      <c r="B237" t="s">
-        <v>513</v>
       </c>
       <c r="C237">
         <v>834</v>
@@ -7522,12 +7519,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A238" t="s">
+        <v>513</v>
+      </c>
+      <c r="B238" t="s">
         <v>514</v>
-      </c>
-      <c r="B238" t="s">
-        <v>515</v>
       </c>
       <c r="C238">
         <v>581</v>
@@ -7542,15 +7539,15 @@
         <v>27</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A239" t="s">
+        <v>515</v>
+      </c>
+      <c r="B239" t="s">
         <v>516</v>
-      </c>
-      <c r="B239" t="s">
-        <v>517</v>
       </c>
       <c r="C239">
         <v>840</v>
@@ -7568,12 +7565,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A240" t="s">
+        <v>517</v>
+      </c>
+      <c r="B240" t="s">
         <v>518</v>
-      </c>
-      <c r="B240" t="s">
-        <v>519</v>
       </c>
       <c r="C240">
         <v>850</v>
@@ -7593,10 +7590,10 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A241" t="s">
+        <v>519</v>
+      </c>
+      <c r="B241" t="s">
         <v>520</v>
-      </c>
-      <c r="B241" t="s">
-        <v>521</v>
       </c>
       <c r="C241">
         <v>858</v>
@@ -7616,10 +7613,10 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A242" t="s">
+        <v>521</v>
+      </c>
+      <c r="B242" t="s">
         <v>522</v>
-      </c>
-      <c r="B242" t="s">
-        <v>523</v>
       </c>
       <c r="C242">
         <v>860</v>
@@ -7639,10 +7636,10 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A243" t="s">
+        <v>523</v>
+      </c>
+      <c r="B243" t="s">
         <v>524</v>
-      </c>
-      <c r="B243" t="s">
-        <v>525</v>
       </c>
       <c r="C243">
         <v>548</v>
@@ -7657,15 +7654,15 @@
         <v>27</v>
       </c>
       <c r="G243" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A244" t="s">
+        <v>525</v>
+      </c>
+      <c r="B244" t="s">
         <v>526</v>
-      </c>
-      <c r="B244" t="s">
-        <v>527</v>
       </c>
       <c r="C244">
         <v>862</v>
@@ -7685,10 +7682,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A245" t="s">
+        <v>527</v>
+      </c>
+      <c r="B245" t="s">
         <v>528</v>
-      </c>
-      <c r="B245" t="s">
-        <v>529</v>
       </c>
       <c r="C245">
         <v>704</v>
@@ -7703,15 +7700,15 @@
         <v>11</v>
       </c>
       <c r="G245" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A246" t="s">
+        <v>529</v>
+      </c>
+      <c r="B246" t="s">
         <v>530</v>
-      </c>
-      <c r="B246" t="s">
-        <v>531</v>
       </c>
       <c r="C246">
         <v>876</v>
@@ -7726,15 +7723,15 @@
         <v>27</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A247" t="s">
+        <v>531</v>
+      </c>
+      <c r="B247" t="s">
         <v>532</v>
-      </c>
-      <c r="B247" t="s">
-        <v>533</v>
       </c>
       <c r="C247">
         <v>732</v>
@@ -7754,10 +7751,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A248" t="s">
+        <v>533</v>
+      </c>
+      <c r="B248" t="s">
         <v>534</v>
-      </c>
-      <c r="B248" t="s">
-        <v>535</v>
       </c>
       <c r="C248">
         <v>887</v>
@@ -7777,10 +7774,10 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A249" t="s">
+        <v>535</v>
+      </c>
+      <c r="B249" t="s">
         <v>536</v>
-      </c>
-      <c r="B249" t="s">
-        <v>537</v>
       </c>
       <c r="C249">
         <v>894</v>
@@ -7800,10 +7797,10 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A250" t="s">
+        <v>537</v>
+      </c>
+      <c r="B250" t="s">
         <v>538</v>
-      </c>
-      <c r="B250" t="s">
-        <v>539</v>
       </c>
       <c r="C250">
         <v>716</v>

</xml_diff>